<commit_message>
[ADD] UK Generation Installed Capacity
</commit_message>
<xml_diff>
--- a/Data/UK Generation Mix.xlsx
+++ b/Data/UK Generation Mix.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectorleduc/Desktop/IMPERIAL COLLEGE LONDON-MSc/Power System Planning/Coursework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Desktop\Imperial College\Spring Term\Power System Planning\PowerSystemPlanning_CW\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CBD22A1-DC5A-2D42-8AEA-C4351A52B9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0E6529-CFC8-422E-98ED-3EC5B55C180C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2340" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{2EDC82A8-379D-454C-BF87-7D61085018C0}"/>
+    <workbookView xWindow="5925" yWindow="-16200" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{2EDC82A8-379D-454C-BF87-7D61085018C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Interconnectors</t>
   </si>
@@ -108,6 +109,24 @@
   </si>
   <si>
     <t>2022 (GW)</t>
+  </si>
+  <si>
+    <t>OffshoreWind</t>
+  </si>
+  <si>
+    <t>OnshoreWind</t>
+  </si>
+  <si>
+    <t>Gas-CT</t>
+  </si>
+  <si>
+    <t>Gas-CC</t>
+  </si>
+  <si>
+    <t>Gen</t>
+  </si>
+  <si>
+    <t>CAP</t>
   </si>
 </sst>
 </file>
@@ -178,13 +197,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -522,16 +543,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7FE727-1391-9441-B3B2-545EC92C79FF}">
   <dimension ref="B1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
@@ -547,12 +568,12 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.5">
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -608,7 +629,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -636,7 +657,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -692,7 +713,7 @@
         <v>151.01512713900954</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -748,7 +769,7 @@
         <v>115.96304680978329</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -804,7 +825,7 @@
         <v>100.9475389330136</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -812,7 +833,7 @@
         <v>42.257346000000005</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -820,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -828,7 +849,7 @@
         <v>14.040748000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -836,7 +857,7 @@
         <v>13.427700000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
@@ -844,7 +865,7 @@
         <v>13.596419000000001</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -852,7 +873,7 @@
         <v>5.2429140000000007</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -860,7 +881,7 @@
         <v>5.2631509999999997</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.5">
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
@@ -868,7 +889,7 @@
         <v>57.7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
@@ -876,7 +897,7 @@
         <v>36.294083000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
@@ -884,13 +905,104 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="4">
         <v>1.723263</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B181183-4E7F-4516-8528-C1F083E577A7}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="25.6875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>8294.0830000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>4240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>14040.748000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>13427.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>13596.419000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="B15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>